<commit_message>
Atualizando a base de dados com o mÊs de agosto
</commit_message>
<xml_diff>
--- a/dezenasSorteadas.xlsx
+++ b/dezenasSorteadas.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\DIO\ETL-Python\PROJETO-NF-PREMIADA-MS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arlei Lissoni\Nota-MS-Premiada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E2ACAB-4EE3-43C1-B5B7-1BE97A6F7246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC6D04B3-F02B-42FF-BDAB-399D79B33B76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$14</definedName>
+  </definedNames>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>04 11 12 44 45 57</t>
   </si>
@@ -70,25 +72,22 @@
   </si>
   <si>
     <t>04 10 12 14 36 46</t>
+  </si>
+  <si>
+    <t>01 19 35 40 47 54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF6E6E6E"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,10 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,20 +426,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24616533-73AD-4497-8D6C-FE5C305AE8EC}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -449,55 +447,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>44378</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+        <v>44013</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>44348</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44044</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>44317</v>
+        <v>44075</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>44287</v>
+        <v>44105</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>44256</v>
+        <v>44136</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>44228</v>
+        <v>44166</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44197</v>
       </c>
@@ -505,55 +503,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>44136</v>
+        <v>44256</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>44105</v>
+        <v>44287</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>44075</v>
+        <v>44317</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>44044</v>
+        <v>44348</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>44013</v>
+        <v>44378</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>44409</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B14">
+    <sortState ref="A2:B14">
+      <sortCondition ref="A1:A14"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>